<commit_message>
Add featured mfcc where are all songs preproccessed and logic in program to handle it
</commit_message>
<xml_diff>
--- a/report/data.xlsx
+++ b/report/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="119">
   <si>
     <t>blues ['country']</t>
   </si>
@@ -727,6 +727,18 @@
       </rPr>
       <t>))</t>
     </r>
+  </si>
+  <si>
+    <t>accuracy:  0.43</t>
+  </si>
+  <si>
+    <t>train_model_minkowski3_new_features</t>
+  </si>
+  <si>
+    <t>accuracy:  0.435</t>
+  </si>
+  <si>
+    <t>train_model_minkowski4_new_features</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AR202"/>
+  <dimension ref="B1:BB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BB1" sqref="BB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,7 +1101,7 @@
     <col min="39" max="39" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
@@ -1114,8 +1126,14 @@
       <c r="AP1" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1140,8 +1158,14 @@
       <c r="AP2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1172,8 +1196,14 @@
       <c r="AP3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1204,8 +1234,14 @@
       <c r="AR4" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX4" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1233,8 +1269,14 @@
       <c r="AP5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1262,8 +1304,14 @@
       <c r="AP6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX6" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -1285,8 +1333,14 @@
       <c r="AP7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX7" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -1308,8 +1362,14 @@
       <c r="AP8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1331,8 +1391,14 @@
       <c r="AP9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1354,8 +1420,14 @@
       <c r="AP10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX10" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -1377,8 +1449,14 @@
       <c r="AP11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX11" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -1400,8 +1478,14 @@
       <c r="AP12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -1423,8 +1507,14 @@
       <c r="AP13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX13" t="s">
+        <v>65</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -1446,8 +1536,14 @@
       <c r="AP14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX14" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -1469,8 +1565,14 @@
       <c r="AP15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="AX15" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>4</v>
       </c>
@@ -1492,8 +1594,14 @@
       <c r="AP16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -1515,8 +1623,14 @@
       <c r="AP17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX17" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -1538,8 +1652,14 @@
       <c r="AP18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX18" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1561,8 +1681,14 @@
       <c r="AP19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX19" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -1584,8 +1710,14 @@
       <c r="AP20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX20" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -1607,8 +1739,14 @@
       <c r="AP21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX21" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -1630,8 +1768,14 @@
       <c r="AP22" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX22" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>6</v>
       </c>
@@ -1653,8 +1797,14 @@
       <c r="AP23" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX23" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1676,8 +1826,14 @@
       <c r="AP24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX24" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>6</v>
       </c>
@@ -1699,8 +1855,14 @@
       <c r="AP25" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX25" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -1722,8 +1884,14 @@
       <c r="AP26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX26" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>6</v>
       </c>
@@ -1745,8 +1913,14 @@
       <c r="AP27" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX27" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>6</v>
       </c>
@@ -1768,8 +1942,14 @@
       <c r="AP28" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX28" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -1791,8 +1971,14 @@
       <c r="AP29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX29" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1814,8 +2000,14 @@
       <c r="AP30" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX30" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -1837,8 +2029,14 @@
       <c r="AP31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX31" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -1860,8 +2058,14 @@
       <c r="AP32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX32" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -1883,8 +2087,14 @@
       <c r="AP33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX33" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -1906,8 +2116,14 @@
       <c r="AP34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX34" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>6</v>
       </c>
@@ -1929,8 +2145,14 @@
       <c r="AP35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX35" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>6</v>
       </c>
@@ -1952,8 +2174,14 @@
       <c r="AP36" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX36" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>6</v>
       </c>
@@ -1975,8 +2203,14 @@
       <c r="AP37" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="38" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX37" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -1998,8 +2232,14 @@
       <c r="AP38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX38" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>6</v>
       </c>
@@ -2021,8 +2261,14 @@
       <c r="AP39" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="40" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX39" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>8</v>
       </c>
@@ -2044,8 +2290,14 @@
       <c r="AP40" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX40" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>6</v>
       </c>
@@ -2067,8 +2319,14 @@
       <c r="AP41" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX41" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>9</v>
       </c>
@@ -2090,8 +2348,14 @@
       <c r="AP42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX42" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>10</v>
       </c>
@@ -2113,8 +2377,14 @@
       <c r="AP43" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX43" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>11</v>
       </c>
@@ -2136,8 +2406,14 @@
       <c r="AP44" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX44" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>12</v>
       </c>
@@ -2159,8 +2435,14 @@
       <c r="AP45" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX45" t="s">
+        <v>12</v>
+      </c>
+      <c r="BB45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>12</v>
       </c>
@@ -2182,8 +2464,14 @@
       <c r="AP46" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX46" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>12</v>
       </c>
@@ -2205,8 +2493,14 @@
       <c r="AP47" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX47" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>13</v>
       </c>
@@ -2228,8 +2522,14 @@
       <c r="AP48" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX48" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>9</v>
       </c>
@@ -2251,8 +2551,14 @@
       <c r="AP49" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX49" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>13</v>
       </c>
@@ -2274,8 +2580,14 @@
       <c r="AP50" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX50" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -2297,8 +2609,14 @@
       <c r="AP51" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX51" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>10</v>
       </c>
@@ -2320,8 +2638,14 @@
       <c r="AP52" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX52" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>11</v>
       </c>
@@ -2343,8 +2667,14 @@
       <c r="AP53" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="54" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX53" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>12</v>
       </c>
@@ -2366,8 +2696,14 @@
       <c r="AP54" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX54" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>15</v>
       </c>
@@ -2389,8 +2725,14 @@
       <c r="AP55" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX55" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>9</v>
       </c>
@@ -2412,8 +2754,14 @@
       <c r="AP56" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX56" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>12</v>
       </c>
@@ -2435,8 +2783,14 @@
       <c r="AP57" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX57" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>16</v>
       </c>
@@ -2458,8 +2812,14 @@
       <c r="AP58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX58" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>14</v>
       </c>
@@ -2481,8 +2841,14 @@
       <c r="AP59" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="60" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX59" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>17</v>
       </c>
@@ -2504,8 +2870,14 @@
       <c r="AP60" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX60" t="s">
+        <v>17</v>
+      </c>
+      <c r="BB60" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>11</v>
       </c>
@@ -2527,8 +2899,14 @@
       <c r="AP61" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="62" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX61" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>18</v>
       </c>
@@ -2550,8 +2928,14 @@
       <c r="AP62" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="63" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX62" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>19</v>
       </c>
@@ -2573,8 +2957,14 @@
       <c r="AP63" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="64" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX63" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>20</v>
       </c>
@@ -2596,8 +2986,14 @@
       <c r="AP64" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX64" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>21</v>
       </c>
@@ -2619,8 +3015,14 @@
       <c r="AP65" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX65" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>18</v>
       </c>
@@ -2642,8 +3044,14 @@
       <c r="AP66" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="67" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX66" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>20</v>
       </c>
@@ -2665,8 +3073,14 @@
       <c r="AP67" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="68" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX67" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>21</v>
       </c>
@@ -2688,8 +3102,14 @@
       <c r="AP68" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="69" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX68" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>20</v>
       </c>
@@ -2711,8 +3131,14 @@
       <c r="AP69" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="70" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX69" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>22</v>
       </c>
@@ -2734,8 +3160,14 @@
       <c r="AP70" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="71" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX70" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>23</v>
       </c>
@@ -2757,8 +3189,14 @@
       <c r="AP71" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="72" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX71" t="s">
+        <v>23</v>
+      </c>
+      <c r="BB71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>20</v>
       </c>
@@ -2780,8 +3218,14 @@
       <c r="AP72" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="73" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX72" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>24</v>
       </c>
@@ -2803,8 +3247,14 @@
       <c r="AP73" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="74" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX73" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB73" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>22</v>
       </c>
@@ -2826,8 +3276,14 @@
       <c r="AP74" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="75" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX74" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB74" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>20</v>
       </c>
@@ -2849,8 +3305,14 @@
       <c r="AP75" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX75" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>22</v>
       </c>
@@ -2872,8 +3334,14 @@
       <c r="AP76" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="77" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX76" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>20</v>
       </c>
@@ -2895,8 +3363,14 @@
       <c r="AP77" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="78" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX77" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>25</v>
       </c>
@@ -2918,8 +3392,14 @@
       <c r="AP78" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="79" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX78" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>19</v>
       </c>
@@ -2941,8 +3421,14 @@
       <c r="AP79" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="80" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX79" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>25</v>
       </c>
@@ -2964,8 +3450,14 @@
       <c r="AP80" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX80" t="s">
+        <v>19</v>
+      </c>
+      <c r="BB80" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>20</v>
       </c>
@@ -2987,8 +3479,14 @@
       <c r="AP81" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="82" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX81" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB81" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>26</v>
       </c>
@@ -3010,8 +3508,14 @@
       <c r="AP82" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="83" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX82" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>27</v>
       </c>
@@ -3033,8 +3537,14 @@
       <c r="AP83" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="84" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX83" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB83" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>27</v>
       </c>
@@ -3056,8 +3566,14 @@
       <c r="AP84" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="85" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX84" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB84" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>26</v>
       </c>
@@ -3079,8 +3595,14 @@
       <c r="AP85" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="86" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX85" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>26</v>
       </c>
@@ -3102,8 +3624,14 @@
       <c r="AP86" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="87" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX86" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB86" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>28</v>
       </c>
@@ -3125,8 +3653,14 @@
       <c r="AP87" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="88" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX87" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>29</v>
       </c>
@@ -3148,8 +3682,14 @@
       <c r="AP88" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="89" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX88" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB88" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>30</v>
       </c>
@@ -3171,8 +3711,14 @@
       <c r="AP89" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="90" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX89" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>28</v>
       </c>
@@ -3194,8 +3740,14 @@
       <c r="AP90" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="91" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX90" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB90" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>31</v>
       </c>
@@ -3217,8 +3769,14 @@
       <c r="AP91" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="92" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX91" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB91" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>26</v>
       </c>
@@ -3240,8 +3798,14 @@
       <c r="AP92" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="93" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX92" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>31</v>
       </c>
@@ -3263,8 +3827,14 @@
       <c r="AP93" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="94" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX93" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB93" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="94" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>28</v>
       </c>
@@ -3286,8 +3856,14 @@
       <c r="AP94" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="95" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX94" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>26</v>
       </c>
@@ -3309,8 +3885,14 @@
       <c r="AP95" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="96" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX95" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>26</v>
       </c>
@@ -3332,8 +3914,14 @@
       <c r="AP96" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="97" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX96" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB96" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="97" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>29</v>
       </c>
@@ -3355,8 +3943,14 @@
       <c r="AP97" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="98" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX97" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB97" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>26</v>
       </c>
@@ -3378,8 +3972,14 @@
       <c r="AP98" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="99" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX98" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB98" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>26</v>
       </c>
@@ -3401,8 +4001,14 @@
       <c r="AP99" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="100" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX99" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB99" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>26</v>
       </c>
@@ -3424,8 +4030,14 @@
       <c r="AP100" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="101" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX100" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>29</v>
       </c>
@@ -3447,8 +4059,14 @@
       <c r="AP101" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="102" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX101" t="s">
+        <v>87</v>
+      </c>
+      <c r="BB101" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="102" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>32</v>
       </c>
@@ -3470,8 +4088,14 @@
       <c r="AP102" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="103" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX102" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB102" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>32</v>
       </c>
@@ -3493,8 +4117,14 @@
       <c r="AP103" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="104" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX103" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB103" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>33</v>
       </c>
@@ -3516,8 +4146,14 @@
       <c r="AP104" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="105" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX104" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB104" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>32</v>
       </c>
@@ -3539,8 +4175,14 @@
       <c r="AP105" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="106" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX105" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB105" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>34</v>
       </c>
@@ -3562,8 +4204,14 @@
       <c r="AP106" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="107" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX106" t="s">
+        <v>101</v>
+      </c>
+      <c r="BB106" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="107" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>33</v>
       </c>
@@ -3585,8 +4233,14 @@
       <c r="AP107" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="108" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX107" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB107" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="108" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>33</v>
       </c>
@@ -3608,8 +4262,14 @@
       <c r="AP108" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="109" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX108" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>35</v>
       </c>
@@ -3631,8 +4291,14 @@
       <c r="AP109" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="110" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX109" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>32</v>
       </c>
@@ -3654,8 +4320,14 @@
       <c r="AP110" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="111" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX110" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB110" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="111" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>35</v>
       </c>
@@ -3677,8 +4349,14 @@
       <c r="AP111" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="112" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX111" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB111" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="112" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>36</v>
       </c>
@@ -3700,8 +4378,14 @@
       <c r="AP112" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="113" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX112" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB112" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>32</v>
       </c>
@@ -3723,8 +4407,14 @@
       <c r="AP113" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="114" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX113" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB113" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>36</v>
       </c>
@@ -3746,8 +4436,14 @@
       <c r="AP114" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="115" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX114" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB114" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="115" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>37</v>
       </c>
@@ -3769,8 +4465,14 @@
       <c r="AP115" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="116" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX115" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB115" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>37</v>
       </c>
@@ -3792,8 +4494,14 @@
       <c r="AP116" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="117" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX116" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB116" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="117" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>33</v>
       </c>
@@ -3815,8 +4523,14 @@
       <c r="AP117" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="118" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX117" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB117" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>37</v>
       </c>
@@ -3838,8 +4552,14 @@
       <c r="AP118" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="119" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX118" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB118" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>35</v>
       </c>
@@ -3861,8 +4581,14 @@
       <c r="AP119" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="120" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX119" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>37</v>
       </c>
@@ -3884,8 +4610,14 @@
       <c r="AP120" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="121" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX120" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB120" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="121" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>33</v>
       </c>
@@ -3907,8 +4639,14 @@
       <c r="AP121" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="122" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX121" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB121" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>38</v>
       </c>
@@ -3930,8 +4668,14 @@
       <c r="AP122" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="123" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX122" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB122" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="123" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>38</v>
       </c>
@@ -3953,8 +4697,14 @@
       <c r="AP123" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="124" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX123" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB123" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>38</v>
       </c>
@@ -3976,8 +4726,14 @@
       <c r="AP124" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="125" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX124" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB124" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>38</v>
       </c>
@@ -3999,8 +4755,14 @@
       <c r="AP125" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="126" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX125" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB125" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="126" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>38</v>
       </c>
@@ -4022,8 +4784,14 @@
       <c r="AP126" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="127" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX126" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB126" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>38</v>
       </c>
@@ -4045,8 +4813,14 @@
       <c r="AP127" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="128" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX127" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB127" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="128" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>38</v>
       </c>
@@ -4068,8 +4842,14 @@
       <c r="AP128" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="129" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX128" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB128" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>39</v>
       </c>
@@ -4091,8 +4871,14 @@
       <c r="AP129" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="130" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX129" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB129" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="130" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>38</v>
       </c>
@@ -4114,8 +4900,14 @@
       <c r="AP130" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="131" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX130" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB130" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>38</v>
       </c>
@@ -4137,8 +4929,14 @@
       <c r="AP131" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="132" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX131" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB131" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>38</v>
       </c>
@@ -4160,8 +4958,14 @@
       <c r="AP132" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="133" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX132" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB132" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="133" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>39</v>
       </c>
@@ -4183,8 +4987,14 @@
       <c r="AP133" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="134" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX133" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB133" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="134" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>40</v>
       </c>
@@ -4206,8 +5016,14 @@
       <c r="AP134" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="135" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX134" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB134" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>38</v>
       </c>
@@ -4229,8 +5045,14 @@
       <c r="AP135" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="136" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX135" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB135" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>38</v>
       </c>
@@ -4252,8 +5074,14 @@
       <c r="AP136" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="137" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX136" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB136" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="137" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>38</v>
       </c>
@@ -4275,8 +5103,14 @@
       <c r="AP137" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="138" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX137" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB137" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="138" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>41</v>
       </c>
@@ -4298,8 +5132,14 @@
       <c r="AP138" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="139" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX138" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB138" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="139" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>42</v>
       </c>
@@ -4321,8 +5161,14 @@
       <c r="AP139" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="140" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX139" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB139" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="140" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>38</v>
       </c>
@@ -4344,8 +5190,14 @@
       <c r="AP140" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="141" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX140" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB140" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="141" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>38</v>
       </c>
@@ -4367,8 +5219,14 @@
       <c r="AP141" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="142" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX141" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB141" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="142" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>43</v>
       </c>
@@ -4390,8 +5248,14 @@
       <c r="AP142" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="143" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX142" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB142" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="143" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>44</v>
       </c>
@@ -4413,8 +5277,14 @@
       <c r="AP143" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="144" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX143" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB143" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="144" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>45</v>
       </c>
@@ -4436,8 +5306,14 @@
       <c r="AP144" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="145" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX144" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB144" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>44</v>
       </c>
@@ -4459,8 +5335,14 @@
       <c r="AP145" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="146" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX145" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB145" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>44</v>
       </c>
@@ -4482,8 +5364,14 @@
       <c r="AP146" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="147" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX146" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB146" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="147" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>45</v>
       </c>
@@ -4505,8 +5393,14 @@
       <c r="AP147" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="148" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX147" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB147" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="148" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>44</v>
       </c>
@@ -4528,8 +5422,14 @@
       <c r="AP148" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="149" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX148" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB148" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>44</v>
       </c>
@@ -4551,8 +5451,14 @@
       <c r="AP149" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="150" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX149" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB149" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="150" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>44</v>
       </c>
@@ -4574,8 +5480,14 @@
       <c r="AP150" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="151" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX150" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB150" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="151" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>46</v>
       </c>
@@ -4597,8 +5509,14 @@
       <c r="AP151" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="152" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX151" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB151" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="152" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>44</v>
       </c>
@@ -4620,8 +5538,14 @@
       <c r="AP152" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="153" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX152" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB152" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="153" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>44</v>
       </c>
@@ -4643,8 +5567,14 @@
       <c r="AP153" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="154" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX153" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB153" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="154" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>47</v>
       </c>
@@ -4666,8 +5596,14 @@
       <c r="AP154" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="155" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX154" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB154" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="155" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>45</v>
       </c>
@@ -4689,8 +5625,14 @@
       <c r="AP155" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="156" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX155" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB155" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="156" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>47</v>
       </c>
@@ -4712,8 +5654,14 @@
       <c r="AP156" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="157" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX156" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB156" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="157" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>47</v>
       </c>
@@ -4735,8 +5683,14 @@
       <c r="AP157" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="158" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX157" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB157" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="158" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>47</v>
       </c>
@@ -4758,8 +5712,14 @@
       <c r="AP158" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="159" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX158" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB158" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="159" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>44</v>
       </c>
@@ -4781,8 +5741,14 @@
       <c r="AP159" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="160" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX159" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB159" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="160" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>45</v>
       </c>
@@ -4804,8 +5770,14 @@
       <c r="AP160" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="161" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX160" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB160" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="161" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>44</v>
       </c>
@@ -4827,8 +5799,14 @@
       <c r="AP161" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="162" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX161" t="s">
+        <v>44</v>
+      </c>
+      <c r="BB161" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="162" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>48</v>
       </c>
@@ -4850,8 +5828,14 @@
       <c r="AP162" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="163" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX162" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB162" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="163" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>49</v>
       </c>
@@ -4873,8 +5857,14 @@
       <c r="AP163" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="164" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX163" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB163" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="164" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>50</v>
       </c>
@@ -4896,8 +5886,14 @@
       <c r="AP164" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="165" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX164" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB164" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="165" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>51</v>
       </c>
@@ -4919,8 +5915,14 @@
       <c r="AP165" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="166" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX165" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB165" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="166" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>50</v>
       </c>
@@ -4942,8 +5944,14 @@
       <c r="AP166" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="167" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX166" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB166" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="167" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>51</v>
       </c>
@@ -4965,8 +5973,14 @@
       <c r="AP167" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="168" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX167" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB167" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="168" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>48</v>
       </c>
@@ -4988,8 +6002,14 @@
       <c r="AP168" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="169" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX168" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB168" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="169" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>50</v>
       </c>
@@ -5011,8 +6031,14 @@
       <c r="AP169" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="170" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX169" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB169" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="170" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>50</v>
       </c>
@@ -5034,8 +6060,14 @@
       <c r="AP170" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="171" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX170" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB170" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="171" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>50</v>
       </c>
@@ -5057,8 +6089,14 @@
       <c r="AP171" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="172" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX171" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB171" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="172" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>50</v>
       </c>
@@ -5080,8 +6118,14 @@
       <c r="AP172" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="173" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX172" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB172" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="173" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>50</v>
       </c>
@@ -5103,8 +6147,14 @@
       <c r="AP173" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="174" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX173" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB173" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="174" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>50</v>
       </c>
@@ -5126,8 +6176,14 @@
       <c r="AP174" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="175" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX174" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB174" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>52</v>
       </c>
@@ -5149,8 +6205,14 @@
       <c r="AP175" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="176" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX175" t="s">
+        <v>49</v>
+      </c>
+      <c r="BB175" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="176" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>52</v>
       </c>
@@ -5172,8 +6234,14 @@
       <c r="AP176" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="177" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX176" t="s">
+        <v>49</v>
+      </c>
+      <c r="BB176" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="177" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>50</v>
       </c>
@@ -5195,8 +6263,14 @@
       <c r="AP177" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="178" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX177" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB177" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>50</v>
       </c>
@@ -5218,8 +6292,14 @@
       <c r="AP178" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="179" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX178" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB178" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="179" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>51</v>
       </c>
@@ -5241,8 +6321,14 @@
       <c r="AP179" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="180" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX179" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB179" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="180" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>50</v>
       </c>
@@ -5264,8 +6350,14 @@
       <c r="AP180" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="181" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX180" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB180" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="181" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>51</v>
       </c>
@@ -5287,8 +6379,14 @@
       <c r="AP181" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="182" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX181" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB181" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="182" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>53</v>
       </c>
@@ -5310,8 +6408,14 @@
       <c r="AP182" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="183" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX182" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB182" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="183" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>54</v>
       </c>
@@ -5333,8 +6437,14 @@
       <c r="AP183" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="184" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX183" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB183" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="184" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>55</v>
       </c>
@@ -5356,8 +6466,14 @@
       <c r="AP184" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="185" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX184" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB184" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="185" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>56</v>
       </c>
@@ -5379,8 +6495,14 @@
       <c r="AP185" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="186" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX185" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB185" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="186" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>56</v>
       </c>
@@ -5402,8 +6524,14 @@
       <c r="AP186" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="187" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX186" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB186" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="187" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>57</v>
       </c>
@@ -5425,8 +6553,14 @@
       <c r="AP187" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="188" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX187" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB187" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="188" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>54</v>
       </c>
@@ -5448,8 +6582,14 @@
       <c r="AP188" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="189" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX188" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB188" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="189" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>57</v>
       </c>
@@ -5471,8 +6611,14 @@
       <c r="AP189" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="190" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX189" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB189" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="190" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>58</v>
       </c>
@@ -5494,8 +6640,14 @@
       <c r="AP190" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="191" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX190" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB190" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="191" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>59</v>
       </c>
@@ -5517,8 +6669,14 @@
       <c r="AP191" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="192" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX191" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB191" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="192" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>57</v>
       </c>
@@ -5540,8 +6698,14 @@
       <c r="AP192" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="193" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX192" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB192" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="193" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>56</v>
       </c>
@@ -5563,8 +6727,14 @@
       <c r="AP193" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="194" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX193" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB193" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="194" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>57</v>
       </c>
@@ -5586,8 +6756,14 @@
       <c r="AP194" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="195" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX194" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB194" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="195" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>57</v>
       </c>
@@ -5609,8 +6785,14 @@
       <c r="AP195" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="196" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX195" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB195" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="196" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>55</v>
       </c>
@@ -5632,8 +6814,14 @@
       <c r="AP196" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="197" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX196" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB196" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="197" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>60</v>
       </c>
@@ -5655,8 +6843,14 @@
       <c r="AP197" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="198" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX197" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB197" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="198" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>61</v>
       </c>
@@ -5678,8 +6872,14 @@
       <c r="AP198" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="199" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX198" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB198" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="199" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>53</v>
       </c>
@@ -5701,8 +6901,14 @@
       <c r="AP199" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="200" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX199" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB199" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="200" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>56</v>
       </c>
@@ -5724,8 +6930,14 @@
       <c r="AP200" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="201" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX200" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB200" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="201" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>53</v>
       </c>
@@ -5747,8 +6959,14 @@
       <c r="AP201" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="202" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="AX201" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB201" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="202" spans="2:54" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>62</v>
       </c>
@@ -5769,6 +6987,12 @@
       </c>
       <c r="AP202" t="s">
         <v>112</v>
+      </c>
+      <c r="AX202" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB202" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New data in report and data
</commit_message>
<xml_diff>
--- a/report/data.xlsx
+++ b/report/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="120">
   <si>
     <t>blues ['country']</t>
   </si>
@@ -739,6 +739,9 @@
   </si>
   <si>
     <t>train_model_minkowski4_new_features</t>
+  </si>
+  <si>
+    <t>chebyshev</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BB202"/>
+  <dimension ref="B1:BF202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BB1" sqref="BB1"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BE16" sqref="BE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1101,7 +1104,7 @@
     <col min="39" max="39" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:54" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
@@ -1132,8 +1135,11 @@
       <c r="BB1" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1164,8 +1170,11 @@
       <c r="BB2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1202,8 +1211,11 @@
       <c r="BB3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1240,8 +1252,11 @@
       <c r="BB4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1275,8 +1290,11 @@
       <c r="BB5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1310,8 +1328,11 @@
       <c r="BB6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -1339,8 +1360,11 @@
       <c r="BB7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -1368,8 +1392,11 @@
       <c r="BB8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1397,8 +1424,11 @@
       <c r="BB9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -1426,8 +1456,11 @@
       <c r="BB10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -1455,8 +1488,11 @@
       <c r="BB11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -1484,8 +1520,11 @@
       <c r="BB12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -1513,8 +1552,11 @@
       <c r="BB13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -1542,8 +1584,11 @@
       <c r="BB14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -1571,8 +1616,11 @@
       <c r="BB15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>4</v>
       </c>
@@ -1600,8 +1648,11 @@
       <c r="BB16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -1629,8 +1680,11 @@
       <c r="BB17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -1658,8 +1712,11 @@
       <c r="BB18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1687,8 +1744,11 @@
       <c r="BB19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -1716,8 +1776,11 @@
       <c r="BB20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -1745,8 +1808,11 @@
       <c r="BB21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -1774,8 +1840,11 @@
       <c r="BB22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>6</v>
       </c>
@@ -1803,8 +1872,11 @@
       <c r="BB23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1832,8 +1904,11 @@
       <c r="BB24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>6</v>
       </c>
@@ -1861,8 +1936,11 @@
       <c r="BB25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -1890,8 +1968,11 @@
       <c r="BB26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>6</v>
       </c>
@@ -1919,8 +2000,11 @@
       <c r="BB27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>6</v>
       </c>
@@ -1948,8 +2032,11 @@
       <c r="BB28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -1977,8 +2064,11 @@
       <c r="BB29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -2006,8 +2096,11 @@
       <c r="BB30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -2035,8 +2128,11 @@
       <c r="BB31" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -2064,8 +2160,11 @@
       <c r="BB32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -2093,8 +2192,11 @@
       <c r="BB33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -2122,8 +2224,11 @@
       <c r="BB34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>6</v>
       </c>
@@ -2151,8 +2256,11 @@
       <c r="BB35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>6</v>
       </c>
@@ -2180,8 +2288,11 @@
       <c r="BB36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>6</v>
       </c>
@@ -2209,8 +2320,11 @@
       <c r="BB37" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -2238,8 +2352,11 @@
       <c r="BB38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>6</v>
       </c>
@@ -2267,8 +2384,11 @@
       <c r="BB39" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>8</v>
       </c>
@@ -2296,8 +2416,11 @@
       <c r="BB40" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>6</v>
       </c>
@@ -2325,8 +2448,11 @@
       <c r="BB41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>9</v>
       </c>
@@ -2354,8 +2480,11 @@
       <c r="BB42" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>10</v>
       </c>
@@ -2383,8 +2512,11 @@
       <c r="BB43" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>11</v>
       </c>
@@ -2412,8 +2544,11 @@
       <c r="BB44" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>12</v>
       </c>
@@ -2441,8 +2576,11 @@
       <c r="BB45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>12</v>
       </c>
@@ -2470,8 +2608,11 @@
       <c r="BB46" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>12</v>
       </c>
@@ -2499,8 +2640,11 @@
       <c r="BB47" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>13</v>
       </c>
@@ -2528,8 +2672,11 @@
       <c r="BB48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="49" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>9</v>
       </c>
@@ -2557,8 +2704,11 @@
       <c r="BB49" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>13</v>
       </c>
@@ -2586,8 +2736,11 @@
       <c r="BB50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -2615,8 +2768,11 @@
       <c r="BB51" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>10</v>
       </c>
@@ -2644,8 +2800,11 @@
       <c r="BB52" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="53" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>11</v>
       </c>
@@ -2673,8 +2832,11 @@
       <c r="BB53" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="54" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>12</v>
       </c>
@@ -2702,8 +2864,11 @@
       <c r="BB54" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>15</v>
       </c>
@@ -2731,8 +2896,11 @@
       <c r="BB55" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>9</v>
       </c>
@@ -2760,8 +2928,11 @@
       <c r="BB56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>12</v>
       </c>
@@ -2789,8 +2960,11 @@
       <c r="BB57" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>16</v>
       </c>
@@ -2818,8 +2992,11 @@
       <c r="BB58" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>14</v>
       </c>
@@ -2847,8 +3024,11 @@
       <c r="BB59" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="60" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>17</v>
       </c>
@@ -2876,8 +3056,11 @@
       <c r="BB60" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF60" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>11</v>
       </c>
@@ -2905,8 +3088,11 @@
       <c r="BB61" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="62" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>18</v>
       </c>
@@ -2934,8 +3120,11 @@
       <c r="BB62" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="63" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>19</v>
       </c>
@@ -2963,8 +3152,11 @@
       <c r="BB63" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>20</v>
       </c>
@@ -2992,8 +3184,11 @@
       <c r="BB64" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="65" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>21</v>
       </c>
@@ -3021,8 +3216,11 @@
       <c r="BB65" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="66" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>18</v>
       </c>
@@ -3050,8 +3248,11 @@
       <c r="BB66" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="67" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>20</v>
       </c>
@@ -3079,8 +3280,11 @@
       <c r="BB67" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="68" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>21</v>
       </c>
@@ -3108,8 +3312,11 @@
       <c r="BB68" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="69" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>20</v>
       </c>
@@ -3137,8 +3344,11 @@
       <c r="BB69" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="70" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>22</v>
       </c>
@@ -3166,8 +3376,11 @@
       <c r="BB70" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="71" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>23</v>
       </c>
@@ -3195,8 +3408,11 @@
       <c r="BB71" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="72" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>20</v>
       </c>
@@ -3224,8 +3440,11 @@
       <c r="BB72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>24</v>
       </c>
@@ -3253,8 +3472,11 @@
       <c r="BB73" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="74" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF73" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>22</v>
       </c>
@@ -3282,8 +3504,11 @@
       <c r="BB74" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="75" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF74" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>20</v>
       </c>
@@ -3311,8 +3536,11 @@
       <c r="BB75" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="76" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>22</v>
       </c>
@@ -3340,8 +3568,11 @@
       <c r="BB76" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="77" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>20</v>
       </c>
@@ -3369,8 +3600,11 @@
       <c r="BB77" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="78" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF77" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>25</v>
       </c>
@@ -3398,8 +3632,11 @@
       <c r="BB78" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="79" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>19</v>
       </c>
@@ -3427,8 +3664,11 @@
       <c r="BB79" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="80" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>25</v>
       </c>
@@ -3456,8 +3696,11 @@
       <c r="BB80" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF80" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>20</v>
       </c>
@@ -3485,8 +3728,11 @@
       <c r="BB81" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="82" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF81" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>26</v>
       </c>
@@ -3514,8 +3760,11 @@
       <c r="BB82" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="83" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>27</v>
       </c>
@@ -3543,8 +3792,11 @@
       <c r="BB83" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="84" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF83" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>27</v>
       </c>
@@ -3572,8 +3824,11 @@
       <c r="BB84" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="85" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF84" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>26</v>
       </c>
@@ -3601,8 +3856,11 @@
       <c r="BB85" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="86" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>26</v>
       </c>
@@ -3630,8 +3888,11 @@
       <c r="BB86" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="87" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF86" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>28</v>
       </c>
@@ -3659,8 +3920,11 @@
       <c r="BB87" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="88" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>29</v>
       </c>
@@ -3688,8 +3952,11 @@
       <c r="BB88" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="89" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF88" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>30</v>
       </c>
@@ -3717,8 +3984,11 @@
       <c r="BB89" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="90" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>28</v>
       </c>
@@ -3746,8 +4016,11 @@
       <c r="BB90" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="91" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF90" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>31</v>
       </c>
@@ -3775,8 +4048,11 @@
       <c r="BB91" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="92" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF91" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>26</v>
       </c>
@@ -3804,8 +4080,11 @@
       <c r="BB92" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="93" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>31</v>
       </c>
@@ -3833,8 +4112,11 @@
       <c r="BB93" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="94" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF93" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>28</v>
       </c>
@@ -3862,8 +4144,11 @@
       <c r="BB94" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="95" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>26</v>
       </c>
@@ -3891,8 +4176,11 @@
       <c r="BB95" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="96" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>26</v>
       </c>
@@ -3920,8 +4208,11 @@
       <c r="BB96" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="97" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="97" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>29</v>
       </c>
@@ -3949,8 +4240,11 @@
       <c r="BB97" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="98" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF97" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>26</v>
       </c>
@@ -3978,8 +4272,11 @@
       <c r="BB98" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="99" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF98" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="99" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>26</v>
       </c>
@@ -4007,8 +4304,11 @@
       <c r="BB99" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="100" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF99" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>26</v>
       </c>
@@ -4036,8 +4336,11 @@
       <c r="BB100" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="101" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>29</v>
       </c>
@@ -4065,8 +4368,11 @@
       <c r="BB101" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="102" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF101" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="102" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>32</v>
       </c>
@@ -4094,8 +4400,11 @@
       <c r="BB102" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="103" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF102" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>32</v>
       </c>
@@ -4123,8 +4432,11 @@
       <c r="BB103" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="104" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF103" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>33</v>
       </c>
@@ -4152,8 +4464,11 @@
       <c r="BB104" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="105" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF104" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>32</v>
       </c>
@@ -4181,8 +4496,11 @@
       <c r="BB105" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="106" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF105" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>34</v>
       </c>
@@ -4210,8 +4528,11 @@
       <c r="BB106" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="107" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF106" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="107" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>33</v>
       </c>
@@ -4239,8 +4560,11 @@
       <c r="BB107" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="108" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF107" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>33</v>
       </c>
@@ -4268,8 +4592,11 @@
       <c r="BB108" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="109" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>35</v>
       </c>
@@ -4297,8 +4624,11 @@
       <c r="BB109" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="110" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF109" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>32</v>
       </c>
@@ -4326,8 +4656,11 @@
       <c r="BB110" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="111" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF110" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="111" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>35</v>
       </c>
@@ -4355,8 +4688,11 @@
       <c r="BB111" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="112" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF111" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="112" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>36</v>
       </c>
@@ -4384,8 +4720,11 @@
       <c r="BB112" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="113" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF112" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>32</v>
       </c>
@@ -4413,8 +4752,11 @@
       <c r="BB113" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="114" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF113" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>36</v>
       </c>
@@ -4442,8 +4784,11 @@
       <c r="BB114" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="115" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF114" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="115" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>37</v>
       </c>
@@ -4471,8 +4816,11 @@
       <c r="BB115" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="116" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF115" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>37</v>
       </c>
@@ -4500,8 +4848,11 @@
       <c r="BB116" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="117" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF116" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>33</v>
       </c>
@@ -4529,8 +4880,11 @@
       <c r="BB117" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="118" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF117" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="118" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>37</v>
       </c>
@@ -4558,8 +4912,11 @@
       <c r="BB118" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="119" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF118" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>35</v>
       </c>
@@ -4587,8 +4944,11 @@
       <c r="BB119" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="120" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>37</v>
       </c>
@@ -4616,8 +4976,11 @@
       <c r="BB120" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="121" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF120" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>33</v>
       </c>
@@ -4645,8 +5008,11 @@
       <c r="BB121" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="122" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF121" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>38</v>
       </c>
@@ -4674,8 +5040,11 @@
       <c r="BB122" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="123" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF122" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="123" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>38</v>
       </c>
@@ -4703,8 +5072,11 @@
       <c r="BB123" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="124" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF123" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>38</v>
       </c>
@@ -4732,8 +5104,11 @@
       <c r="BB124" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="125" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF124" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>38</v>
       </c>
@@ -4761,8 +5136,11 @@
       <c r="BB125" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="126" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF125" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="126" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>38</v>
       </c>
@@ -4790,8 +5168,11 @@
       <c r="BB126" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="127" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF126" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>38</v>
       </c>
@@ -4819,8 +5200,11 @@
       <c r="BB127" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="128" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF127" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>38</v>
       </c>
@@ -4848,8 +5232,11 @@
       <c r="BB128" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="129" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF128" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>39</v>
       </c>
@@ -4877,8 +5264,11 @@
       <c r="BB129" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="130" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF129" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="130" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>38</v>
       </c>
@@ -4906,8 +5296,11 @@
       <c r="BB130" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="131" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF130" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>38</v>
       </c>
@@ -4935,8 +5328,11 @@
       <c r="BB131" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="132" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF131" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>38</v>
       </c>
@@ -4964,8 +5360,11 @@
       <c r="BB132" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="133" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF132" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>39</v>
       </c>
@@ -4993,8 +5392,11 @@
       <c r="BB133" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="134" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF133" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="134" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>40</v>
       </c>
@@ -5022,8 +5424,11 @@
       <c r="BB134" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="135" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF134" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="135" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>38</v>
       </c>
@@ -5051,8 +5456,11 @@
       <c r="BB135" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="136" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF135" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>38</v>
       </c>
@@ -5080,8 +5488,11 @@
       <c r="BB136" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="137" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF136" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="137" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>38</v>
       </c>
@@ -5109,8 +5520,11 @@
       <c r="BB137" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="138" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF137" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="138" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>41</v>
       </c>
@@ -5138,8 +5552,11 @@
       <c r="BB138" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="139" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF138" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="139" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>42</v>
       </c>
@@ -5167,8 +5584,11 @@
       <c r="BB139" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="140" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF139" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="140" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>38</v>
       </c>
@@ -5196,8 +5616,11 @@
       <c r="BB140" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="141" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF140" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="141" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>38</v>
       </c>
@@ -5225,8 +5648,11 @@
       <c r="BB141" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="142" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF141" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="142" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>43</v>
       </c>
@@ -5254,8 +5680,11 @@
       <c r="BB142" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="143" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF142" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="143" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>44</v>
       </c>
@@ -5283,8 +5712,11 @@
       <c r="BB143" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="144" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF143" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="144" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>45</v>
       </c>
@@ -5312,8 +5744,11 @@
       <c r="BB144" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="145" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF144" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>44</v>
       </c>
@@ -5341,8 +5776,11 @@
       <c r="BB145" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="146" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF145" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>44</v>
       </c>
@@ -5370,8 +5808,11 @@
       <c r="BB146" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="147" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF146" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="147" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>45</v>
       </c>
@@ -5399,8 +5840,11 @@
       <c r="BB147" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="148" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF147" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="148" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>44</v>
       </c>
@@ -5428,8 +5872,11 @@
       <c r="BB148" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="149" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF148" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>44</v>
       </c>
@@ -5457,8 +5904,11 @@
       <c r="BB149" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="150" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF149" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="150" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>44</v>
       </c>
@@ -5486,8 +5936,11 @@
       <c r="BB150" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="151" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF150" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="151" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>46</v>
       </c>
@@ -5515,8 +5968,11 @@
       <c r="BB151" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="152" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF151" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="152" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>44</v>
       </c>
@@ -5544,8 +6000,11 @@
       <c r="BB152" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="153" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF152" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="153" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>44</v>
       </c>
@@ -5573,8 +6032,11 @@
       <c r="BB153" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="154" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF153" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="154" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>47</v>
       </c>
@@ -5602,8 +6064,11 @@
       <c r="BB154" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="155" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF154" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="155" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>45</v>
       </c>
@@ -5631,8 +6096,11 @@
       <c r="BB155" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="156" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF155" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="156" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>47</v>
       </c>
@@ -5660,8 +6128,11 @@
       <c r="BB156" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="157" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF156" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="157" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>47</v>
       </c>
@@ -5689,8 +6160,11 @@
       <c r="BB157" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="158" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF157" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="158" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>47</v>
       </c>
@@ -5718,8 +6192,11 @@
       <c r="BB158" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="159" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF158" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="159" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>44</v>
       </c>
@@ -5747,8 +6224,11 @@
       <c r="BB159" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="160" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF159" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="160" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>45</v>
       </c>
@@ -5776,8 +6256,11 @@
       <c r="BB160" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="161" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF160" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="161" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>44</v>
       </c>
@@ -5805,8 +6288,11 @@
       <c r="BB161" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="162" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF161" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="162" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>48</v>
       </c>
@@ -5834,8 +6320,11 @@
       <c r="BB162" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="163" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF162" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="163" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>49</v>
       </c>
@@ -5863,8 +6352,11 @@
       <c r="BB163" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="164" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF163" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="164" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>50</v>
       </c>
@@ -5892,8 +6384,11 @@
       <c r="BB164" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="165" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF164" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="165" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>51</v>
       </c>
@@ -5921,8 +6416,11 @@
       <c r="BB165" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="166" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF165" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="166" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>50</v>
       </c>
@@ -5950,8 +6448,11 @@
       <c r="BB166" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="167" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF166" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="167" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>51</v>
       </c>
@@ -5979,8 +6480,11 @@
       <c r="BB167" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="168" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF167" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="168" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>48</v>
       </c>
@@ -6008,8 +6512,11 @@
       <c r="BB168" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="169" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF168" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="169" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>50</v>
       </c>
@@ -6037,8 +6544,11 @@
       <c r="BB169" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="170" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF169" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="170" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>50</v>
       </c>
@@ -6066,8 +6576,11 @@
       <c r="BB170" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="171" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF170" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="171" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>50</v>
       </c>
@@ -6095,8 +6608,11 @@
       <c r="BB171" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="172" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF171" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="172" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>50</v>
       </c>
@@ -6124,8 +6640,11 @@
       <c r="BB172" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="173" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF172" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="173" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>50</v>
       </c>
@@ -6153,8 +6672,11 @@
       <c r="BB173" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="174" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF173" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="174" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>50</v>
       </c>
@@ -6182,8 +6704,11 @@
       <c r="BB174" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="175" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF174" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>52</v>
       </c>
@@ -6211,8 +6736,11 @@
       <c r="BB175" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="176" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF175" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="176" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>52</v>
       </c>
@@ -6240,8 +6768,11 @@
       <c r="BB176" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="177" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF176" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="177" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>50</v>
       </c>
@@ -6269,8 +6800,11 @@
       <c r="BB177" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="178" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF177" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>50</v>
       </c>
@@ -6298,8 +6832,11 @@
       <c r="BB178" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="179" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF178" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="179" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>51</v>
       </c>
@@ -6327,8 +6864,11 @@
       <c r="BB179" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="180" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF179" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="180" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>50</v>
       </c>
@@ -6356,8 +6896,11 @@
       <c r="BB180" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="181" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF180" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="181" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>51</v>
       </c>
@@ -6385,8 +6928,11 @@
       <c r="BB181" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="182" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF181" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="182" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>53</v>
       </c>
@@ -6414,8 +6960,11 @@
       <c r="BB182" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="183" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF182" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="183" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>54</v>
       </c>
@@ -6443,8 +6992,11 @@
       <c r="BB183" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="184" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF183" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="184" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>55</v>
       </c>
@@ -6472,8 +7024,11 @@
       <c r="BB184" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="185" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF184" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="185" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>56</v>
       </c>
@@ -6501,8 +7056,11 @@
       <c r="BB185" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="186" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF185" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="186" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>56</v>
       </c>
@@ -6530,8 +7088,11 @@
       <c r="BB186" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="187" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF186" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="187" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>57</v>
       </c>
@@ -6559,8 +7120,11 @@
       <c r="BB187" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="188" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF187" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="188" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>54</v>
       </c>
@@ -6588,8 +7152,11 @@
       <c r="BB188" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="189" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF188" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="189" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>57</v>
       </c>
@@ -6617,8 +7184,11 @@
       <c r="BB189" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="190" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF189" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="190" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>58</v>
       </c>
@@ -6646,8 +7216,11 @@
       <c r="BB190" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="191" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF190" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="191" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>59</v>
       </c>
@@ -6675,8 +7248,11 @@
       <c r="BB191" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="192" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF191" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="192" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>57</v>
       </c>
@@ -6704,8 +7280,11 @@
       <c r="BB192" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="193" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF192" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="193" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>56</v>
       </c>
@@ -6733,8 +7312,11 @@
       <c r="BB193" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="194" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF193" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="194" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>57</v>
       </c>
@@ -6762,8 +7344,11 @@
       <c r="BB194" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="195" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF194" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="195" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>57</v>
       </c>
@@ -6791,8 +7376,11 @@
       <c r="BB195" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="196" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF195" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="196" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>55</v>
       </c>
@@ -6820,8 +7408,11 @@
       <c r="BB196" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="197" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF196" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="197" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>60</v>
       </c>
@@ -6849,8 +7440,11 @@
       <c r="BB197" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="198" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF197" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="198" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>61</v>
       </c>
@@ -6878,8 +7472,11 @@
       <c r="BB198" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="199" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF198" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="199" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>53</v>
       </c>
@@ -6907,8 +7504,11 @@
       <c r="BB199" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="200" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF199" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="200" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>56</v>
       </c>
@@ -6936,8 +7536,11 @@
       <c r="BB200" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="201" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF200" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="201" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>53</v>
       </c>
@@ -6965,8 +7568,11 @@
       <c r="BB201" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="202" spans="2:54" x14ac:dyDescent="0.2">
+      <c r="BF201" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="202" spans="2:58" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>62</v>
       </c>
@@ -6993,6 +7599,9 @@
       </c>
       <c r="BB202" t="s">
         <v>117</v>
+      </c>
+      <c r="BF202" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>